<commit_message>
fix response and password generator while upload data siswa
</commit_message>
<xml_diff>
--- a/server/src/public/siswa.xlsx
+++ b/server/src/public/siswa.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>siswa_nis</t>
   </si>
@@ -42,25 +42,19 @@
     <t>d_kelas_id</t>
   </si>
   <si>
-    <t>sarwer</t>
-  </si>
-  <si>
-    <t>21edwq</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>profile.png</t>
   </si>
   <si>
-    <t>Raka</t>
-  </si>
-  <si>
-    <t>Ade</t>
-  </si>
-  <si>
-    <t>Rafly</t>
+    <t>Asti</t>
+  </si>
+  <si>
+    <t>Damah</t>
+  </si>
+  <si>
+    <t>Anis</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
@@ -463,19 +457,16 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>99028129</v>
+        <v>990229</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="C2">
-        <v>1234</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F2">
         <v>3</v>
@@ -489,19 +480,16 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>200</v>
+        <v>921200</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -515,19 +503,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>300</v>
+        <v>231213</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F4">
         <v>3</v>

</xml_diff>

<commit_message>
update fitur upload siswa with excel
</commit_message>
<xml_diff>
--- a/server/src/public/siswa.xlsx
+++ b/server/src/public/siswa.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>siswa_nis</t>
   </si>
@@ -24,37 +24,46 @@
     <t>siswa_nama</t>
   </si>
   <si>
-    <t>siswa_password</t>
-  </si>
-  <si>
     <t>siswa_gender</t>
   </si>
   <si>
-    <t>siswa_img</t>
-  </si>
-  <si>
-    <t>kelas_id</t>
-  </si>
-  <si>
-    <t>jurusan_id</t>
-  </si>
-  <si>
-    <t>d_kelas_id</t>
-  </si>
-  <si>
-    <t>profile.png</t>
-  </si>
-  <si>
-    <t>Asti</t>
-  </si>
-  <si>
-    <t>Damah</t>
-  </si>
-  <si>
-    <t>Anis</t>
-  </si>
-  <si>
-    <t>P</t>
+    <t>Raka</t>
+  </si>
+  <si>
+    <t>Varits</t>
+  </si>
+  <si>
+    <t>Abel</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>nama_jurusan</t>
+  </si>
+  <si>
+    <t>RPL</t>
+  </si>
+  <si>
+    <t>TKJ</t>
+  </si>
+  <si>
+    <t>kelas</t>
+  </si>
+  <si>
+    <t>d_kelas</t>
+  </si>
+  <si>
+    <t>XII</t>
+  </si>
+  <si>
+    <t>XI</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>TEI</t>
   </si>
 </sst>
 </file>
@@ -107,17 +116,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H4" totalsRowShown="0">
-  <autoFilter ref="A1:H4"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:F10" totalsRowShown="0">
+  <autoFilter ref="A1:F10"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="siswa_nis"/>
     <tableColumn id="2" name="siswa_nama"/>
-    <tableColumn id="3" name="siswa_password"/>
     <tableColumn id="4" name="siswa_gender"/>
-    <tableColumn id="5" name="siswa_img"/>
-    <tableColumn id="6" name="kelas_id"/>
-    <tableColumn id="7" name="jurusan_id"/>
-    <tableColumn id="8" name="d_kelas_id"/>
+    <tableColumn id="6" name="kelas"/>
+    <tableColumn id="7" name="nama_jurusan"/>
+    <tableColumn id="8" name="d_kelas"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -410,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,14 +429,14 @@
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,88 +447,73 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="C2" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>990229</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>921200</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
       <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3">
         <v>1</v>
       </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>231213</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>